<commit_message>
Finished BLE BOM for Three Modules
</commit_message>
<xml_diff>
--- a/Steering/Hardware/BOM/Bluetooth_Module_BOM.xlsx
+++ b/Steering/Hardware/BOM/Bluetooth_Module_BOM.xlsx
@@ -8,17 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\files.auckland.ac.nz\myhome\Desktop\Electeng\2020-srw-rc-car\Steering\Hardware\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52844CB2-589F-4D76-8D35-8EC3FDFC588E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931C8ED2-7886-4E89-AFBD-1CFBCC5E11D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" xr2:uid="{4895F57E-8DCF-4A6C-9607-D9B5352DA2F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -641,7 +646,7 @@
   <dimension ref="B2:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>